<commit_message>
Latitude and Longitude swap
</commit_message>
<xml_diff>
--- a/resources/excel/coderdojo2020.xlsx
+++ b/resources/excel/coderdojo2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\codeweek\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C88AC-9F04-48DA-86F2-E896923D2D1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C6A5F6-C9AE-4A7E-BD4C-48E79DD3EAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18990" yWindow="1530" windowWidth="22095" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1116,8 +1116,8 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K9" sqref="K9"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1173,10 +1173,10 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>13</v>

</xml_diff>